<commit_message>
updated suspense logic UEFA
updating suspense logic for eu uefa goals
</commit_message>
<xml_diff>
--- a/data/out/wiki/men/uefa/eu/tab_prob_eu_uefa.xlsx
+++ b/data/out/wiki/men/uefa/eu/tab_prob_eu_uefa.xlsx
@@ -14524,19 +14524,19 @@
         <v>0.9900878193274961</v>
       </c>
       <c r="K262">
-        <v>-2.419626224819948E-05</v>
+        <v>-2.419626224819948e-05</v>
       </c>
       <c r="L262">
         <v>0</v>
       </c>
       <c r="M262">
-        <v>2.419626224814397E-05</v>
+        <v>2.419626224814397e-05</v>
       </c>
       <c r="N262">
-        <v>2.419626224819948E-05</v>
+        <v>2.419626224819948e-05</v>
       </c>
       <c r="O262">
-        <v>4.839252449634346E-05</v>
+        <v>4.839252449634346e-05</v>
       </c>
       <c r="P262">
         <v>0.0007996535023334433</v>
@@ -14577,19 +14577,19 @@
         <v>0.9900954711035846</v>
       </c>
       <c r="K263">
-        <v>-7.651776088583168E-06</v>
+        <v>-7.651776088583168e-06</v>
       </c>
       <c r="L263">
         <v>0</v>
       </c>
       <c r="M263">
-        <v>7.651776088524187E-06</v>
+        <v>7.651776088524187e-06</v>
       </c>
       <c r="N263">
-        <v>7.651776088583168E-06</v>
+        <v>7.651776088583168e-06</v>
       </c>
       <c r="O263">
-        <v>1.530355217710735E-05</v>
+        <v>1.530355217710735e-05</v>
       </c>
       <c r="P263">
         <v>0.0007990423795652558</v>

</xml_diff>